<commit_message>
Revised Gantt Chart and activity definition estimation
</commit_message>
<xml_diff>
--- a/Gantt_chart.xlsx
+++ b/Gantt_chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j_knz\Documents\Uni\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\Documents\Griffith\localRepo\Milestone1_Group39\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA1ED3B-1FF3-4CE2-B5C8-66A6B6B324FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9BD731-45EE-48CB-A0FA-6933FD3D3CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>PERIODS</t>
   </si>
@@ -198,18 +198,6 @@
     <t>Activity No. and Name</t>
   </si>
   <si>
-    <t>Collect Data</t>
-  </si>
-  <si>
-    <t>Create Scope</t>
-  </si>
-  <si>
-    <t>Conduct User Research</t>
-  </si>
-  <si>
-    <t>Map User Flow</t>
-  </si>
-  <si>
     <t>Design Screen Wireframes</t>
   </si>
   <si>
@@ -262,13 +250,31 @@
   </si>
   <si>
     <t>Food Nutrition Breakdown App</t>
+  </si>
+  <si>
+    <t>1.1 Collect Data</t>
+  </si>
+  <si>
+    <t>1.2 Create Project Plan</t>
+  </si>
+  <si>
+    <t>1.3 Create WBS and schedule</t>
+  </si>
+  <si>
+    <t>1.4 Conduct user research</t>
+  </si>
+  <si>
+    <t>1.5 Create Software Design Document</t>
+  </si>
+  <si>
+    <t>1.6 Map User Flow</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -377,6 +383,14 @@
       <color theme="1" tint="0.24994659260841701"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="8">
@@ -638,12 +652,27 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="10" applyFont="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="10" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -665,22 +694,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="10" applyFont="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1083,28 +1097,28 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BO39"/>
+  <dimension ref="B1:BO41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="CP41" sqref="CP41"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="2.73046875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="2.58203125" customWidth="1"/>
-    <col min="2" max="2" width="21.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="6.58203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.25" style="1" customWidth="1"/>
-    <col min="5" max="5" width="5.75" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6.75" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.59765625" customWidth="1"/>
+    <col min="2" max="2" width="21.46484375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="6.59765625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.265625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="5.73046875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.73046875" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.33203125" style="4" customWidth="1"/>
-    <col min="8" max="27" width="2.75" style="1"/>
-    <col min="42" max="42" width="2.75" customWidth="1"/>
+    <col min="8" max="27" width="2.73046875" style="1"/>
+    <col min="42" max="42" width="2.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.25">
+    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.6">
       <c r="B1" s="11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
@@ -1112,50 +1126,50 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="2:67" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+    <row r="2" spans="2:67" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
       <c r="G2" s="21" t="s">
         <v>25</v>
       </c>
       <c r="H2" s="12">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J2" s="13"/>
-      <c r="K2" s="26" t="s">
+      <c r="K2" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="28"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="33"/>
       <c r="P2" s="14"/>
-      <c r="Q2" s="26" t="s">
+      <c r="Q2" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="28"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="33"/>
       <c r="U2" s="15"/>
-      <c r="V2" s="30" t="s">
+      <c r="V2" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="32"/>
+      <c r="W2" s="36"/>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="37"/>
       <c r="Z2" s="16"/>
-      <c r="AA2" s="30" t="s">
+      <c r="AA2" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="AB2" s="31"/>
-      <c r="AC2" s="31"/>
-      <c r="AD2" s="31"/>
-      <c r="AE2" s="31"/>
-      <c r="AF2" s="31"/>
-      <c r="AG2" s="32"/>
+      <c r="AB2" s="36"/>
+      <c r="AC2" s="36"/>
+      <c r="AD2" s="36"/>
+      <c r="AE2" s="36"/>
+      <c r="AF2" s="36"/>
+      <c r="AG2" s="37"/>
       <c r="AH2" s="17"/>
       <c r="AI2" s="19" t="s">
         <v>8</v>
@@ -1168,23 +1182,23 @@
       <c r="AO2" s="20"/>
       <c r="AP2" s="20"/>
     </row>
-    <row r="3" spans="2:67" s="9" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="34" t="s">
+    <row r="3" spans="2:67" s="9" customFormat="1" ht="40.049999999999997" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="30" t="s">
         <v>24</v>
       </c>
       <c r="H3" s="18" t="s">
@@ -1210,13 +1224,13 @@
       <c r="Z3" s="8"/>
       <c r="AA3" s="8"/>
     </row>
-    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="35"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
+    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="27"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1398,9 +1412,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="37" t="s">
-        <v>27</v>
+    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B5" s="24" t="s">
+        <v>45</v>
       </c>
       <c r="C5" s="5">
         <v>1</v>
@@ -1408,133 +1422,165 @@
       <c r="D5" s="5">
         <v>1</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+      <c r="E5" s="5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5">
+        <v>1</v>
+      </c>
       <c r="G5" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="37" t="s">
-        <v>29</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B6" s="24" t="s">
+        <v>46</v>
       </c>
       <c r="C6" s="5">
         <v>1</v>
       </c>
       <c r="D6" s="5">
-        <v>1</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="E6" s="5">
+        <v>1</v>
+      </c>
+      <c r="F6" s="5">
+        <v>3</v>
+      </c>
       <c r="G6" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B7" s="38" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="C7" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="5">
         <v>1</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="E7" s="5">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5">
+        <v>1</v>
+      </c>
       <c r="G7" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="37" t="s">
-        <v>30</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B8" s="38" t="s">
+        <v>48</v>
       </c>
       <c r="C8" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="5">
         <v>1</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="E8" s="5">
+        <v>1</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1</v>
+      </c>
       <c r="G8" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="37" t="s">
-        <v>31</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B9" s="38" t="s">
+        <v>49</v>
       </c>
       <c r="C9" s="5">
         <v>3</v>
       </c>
       <c r="D9" s="5">
+        <v>4</v>
+      </c>
+      <c r="E9" s="5">
+        <v>3</v>
+      </c>
+      <c r="F9" s="5">
+        <v>4</v>
+      </c>
+      <c r="G9" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B10" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="5">
+        <v>3</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5">
+        <v>3</v>
+      </c>
+      <c r="F10" s="5">
         <v>2</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="5">
+      <c r="G10" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B11" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="5">
+        <v>4</v>
+      </c>
+      <c r="D11" s="5">
+        <v>2</v>
+      </c>
+      <c r="E11" s="5">
+        <v>4</v>
+      </c>
+      <c r="F11" s="5">
+        <v>2</v>
+      </c>
+      <c r="G11" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B12" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="5">
         <v>5</v>
       </c>
-      <c r="D10" s="5">
-        <v>1</v>
-      </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="5">
+      <c r="D12" s="5">
+        <v>1</v>
+      </c>
+      <c r="E12" s="5">
+        <v>5</v>
+      </c>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
+      <c r="G12" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B13" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="5">
         <v>6</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D13" s="5">
         <v>3</v>
-      </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="5">
-        <v>9</v>
-      </c>
-      <c r="D12" s="5">
-        <v>3</v>
-      </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="5">
-        <v>9</v>
-      </c>
-      <c r="D13" s="5">
-        <v>2</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -1542,15 +1588,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="37" t="s">
-        <v>36</v>
+    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B14" s="24" t="s">
+        <v>30</v>
       </c>
       <c r="C14" s="5">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D14" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -1558,15 +1604,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="6">
-        <v>14</v>
+    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B15" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="5">
+        <v>9</v>
       </c>
       <c r="D15" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -1574,12 +1620,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="37" t="s">
-        <v>38</v>
+    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B16" s="24" t="s">
+        <v>32</v>
       </c>
       <c r="C16" s="5">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D16" s="5">
         <v>2</v>
@@ -1590,15 +1636,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="5">
-        <v>20</v>
+    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B17" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="6">
+        <v>14</v>
       </c>
       <c r="D17" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -1606,12 +1652,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="37" t="s">
-        <v>40</v>
+    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B18" s="24" t="s">
+        <v>34</v>
       </c>
       <c r="C18" s="5">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D18" s="5">
         <v>3</v>
@@ -1622,15 +1668,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="37" t="s">
-        <v>41</v>
+    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B19" s="24" t="s">
+        <v>35</v>
       </c>
       <c r="C19" s="5">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D19" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -1638,15 +1684,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="37" t="s">
-        <v>42</v>
+    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B20" s="24" t="s">
+        <v>36</v>
       </c>
       <c r="C20" s="5">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D20" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -1654,12 +1700,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="37" t="s">
-        <v>43</v>
+    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B21" s="24" t="s">
+        <v>37</v>
       </c>
       <c r="C21" s="5">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D21" s="5">
         <v>1</v>
@@ -1670,15 +1716,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="37" t="s">
-        <v>44</v>
+    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B22" s="24" t="s">
+        <v>38</v>
       </c>
       <c r="C22" s="5">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D22" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -1686,15 +1732,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="37" t="s">
-        <v>46</v>
+    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B23" s="24" t="s">
+        <v>39</v>
       </c>
       <c r="C23" s="5">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D23" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -1702,12 +1748,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="37" t="s">
-        <v>45</v>
+    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B24" s="24" t="s">
+        <v>40</v>
       </c>
       <c r="C24" s="5">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D24" s="5">
         <v>3</v>
@@ -1718,12 +1764,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="37" t="s">
-        <v>47</v>
+    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B25" s="24" t="s">
+        <v>42</v>
       </c>
       <c r="C25" s="5">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D25" s="5">
         <v>2</v>
@@ -1734,33 +1780,41 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
+    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B26" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="5">
+        <v>30</v>
+      </c>
+      <c r="D26" s="5">
+        <v>3</v>
+      </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="23" t="s">
+    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B27" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="5">
+        <v>33</v>
+      </c>
+      <c r="D27" s="5">
         <v>2</v>
       </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B28" s="23" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -1770,9 +1824,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B29" s="23" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -1782,9 +1836,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B30" s="23" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -1794,9 +1848,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B31" s="23" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -1806,9 +1860,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B32" s="23" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -1818,9 +1872,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B33" s="23" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -1830,9 +1884,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B34" s="23" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -1842,9 +1896,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B35" s="23" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -1854,9 +1908,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B36" s="23" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -1866,9 +1920,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B37" s="23" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -1878,9 +1932,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B38" s="23" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -1890,9 +1944,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B39" s="23" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -1902,26 +1956,50 @@
         <v>0</v>
       </c>
     </row>
+    <row r="40" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B40" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B41" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:BO4">
     <cfRule type="expression" dxfId="8" priority="8">
       <formula>H$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:BO39">
+  <conditionalFormatting sqref="H5:BO41">
     <cfRule type="expression" dxfId="7" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>

</xml_diff>

<commit_message>
Forgot to add the actual picture of the revised Gantt Chart lol
</commit_message>
<xml_diff>
--- a/Gantt_chart.xlsx
+++ b/Gantt_chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\Documents\Griffith\localRepo\Milestone1_Group39\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9BD731-45EE-48CB-A0FA-6933FD3D3CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19AA2FD-858B-4D05-83C7-09F297326F29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43080" yWindow="1515" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -198,57 +198,6 @@
     <t>Activity No. and Name</t>
   </si>
   <si>
-    <t>Design Screen Wireframes</t>
-  </si>
-  <si>
-    <t>Validate Wireframes</t>
-  </si>
-  <si>
-    <t>Develop User Interface</t>
-  </si>
-  <si>
-    <t>Develop Screen Interconnectivity</t>
-  </si>
-  <si>
-    <t>Implement Provided Database</t>
-  </si>
-  <si>
-    <t>Implement Food Search Feature</t>
-  </si>
-  <si>
-    <t>Implement Nutrition Breakdown Feature</t>
-  </si>
-  <si>
-    <t>Implement Nutrition Range Feature</t>
-  </si>
-  <si>
-    <t>Implement Nutrition Level Filter</t>
-  </si>
-  <si>
-    <t>Implement Dietary Level Filter</t>
-  </si>
-  <si>
-    <t>Unit Testing</t>
-  </si>
-  <si>
-    <t>Alpha Testing</t>
-  </si>
-  <si>
-    <t>Acceptance Testing</t>
-  </si>
-  <si>
-    <t>Fix Bugs</t>
-  </si>
-  <si>
-    <t>Enhance Features</t>
-  </si>
-  <si>
-    <t>Gather Feedback</t>
-  </si>
-  <si>
-    <t>Sanity Test</t>
-  </si>
-  <si>
     <t>Food Nutrition Breakdown App</t>
   </si>
   <si>
@@ -268,6 +217,57 @@
   </si>
   <si>
     <t>1.6 Map User Flow</t>
+  </si>
+  <si>
+    <t>1.7 Design Screen Wireframes</t>
+  </si>
+  <si>
+    <t>1.8 Validate Wireframes</t>
+  </si>
+  <si>
+    <t>2.1 Develop User Interface</t>
+  </si>
+  <si>
+    <t>2.2 Develop Screen Interconnectivity</t>
+  </si>
+  <si>
+    <t>2.3 Implement Provided Database</t>
+  </si>
+  <si>
+    <t>2.4 Implement Food Search Feature</t>
+  </si>
+  <si>
+    <t>2.5 Implement Nutrition Breakdown Feature</t>
+  </si>
+  <si>
+    <t>2.6 Implement Nutrition Range Feature</t>
+  </si>
+  <si>
+    <t>2.7 Implement Nutrition Level Filter</t>
+  </si>
+  <si>
+    <t>2.8 Implement Dietary Level Filter</t>
+  </si>
+  <si>
+    <t>3.1 Unit Testing</t>
+  </si>
+  <si>
+    <t>3.2 Alpha Testing</t>
+  </si>
+  <si>
+    <t>3.3 Acceptance Testing</t>
+  </si>
+  <si>
+    <t>4.1 Fix Bugs</t>
+  </si>
+  <si>
+    <t>4.2 Gather Feedback</t>
+  </si>
+  <si>
+    <t>4.3 Enhance Features</t>
+  </si>
+  <si>
+    <t>4.4 Sanity Test</t>
   </si>
 </sst>
 </file>
@@ -309,6 +309,7 @@
       <sz val="12"/>
       <color theme="1" tint="0.24994659260841701"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -655,6 +656,36 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="10" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="12">
       <alignment vertical="center"/>
     </xf>
@@ -666,36 +697,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="10" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="10" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1099,8 +1100,8 @@
   </sheetPr>
   <dimension ref="B1:BO41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="X9" sqref="X9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="CJ1" sqref="CJ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.73046875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -1112,13 +1113,32 @@
     <col min="5" max="5" width="5.73046875" style="1" customWidth="1"/>
     <col min="6" max="6" width="6.73046875" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.33203125" style="4" customWidth="1"/>
-    <col min="8" max="27" width="2.73046875" style="1"/>
-    <col min="42" max="42" width="2.73046875" customWidth="1"/>
+    <col min="8" max="14" width="2.73046875" style="1"/>
+    <col min="15" max="16" width="2.73046875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="3.9296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.53125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="26" width="3.9296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3.9296875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="4.19921875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="4.19921875" customWidth="1"/>
+    <col min="31" max="34" width="4.19921875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="4.06640625" customWidth="1"/>
+    <col min="36" max="37" width="4.19921875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="3.9296875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="4.19921875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="4.19921875" customWidth="1"/>
+    <col min="41" max="47" width="4.19921875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="3.9296875" bestFit="1" customWidth="1"/>
+    <col min="49" max="57" width="4.19921875" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="3.9296875" bestFit="1" customWidth="1"/>
+    <col min="59" max="67" width="4.19921875" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="2.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.6">
       <c r="B1" s="11" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
@@ -1127,11 +1147,11 @@
       <c r="G1" s="10"/>
     </row>
     <row r="2" spans="2:67" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
       <c r="G2" s="21" t="s">
         <v>25</v>
       </c>
@@ -1139,37 +1159,37 @@
         <v>6</v>
       </c>
       <c r="J2" s="13"/>
-      <c r="K2" s="31" t="s">
+      <c r="K2" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="33"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="30"/>
       <c r="P2" s="14"/>
-      <c r="Q2" s="31" t="s">
+      <c r="Q2" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="33"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="30"/>
       <c r="U2" s="15"/>
-      <c r="V2" s="35" t="s">
+      <c r="V2" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="W2" s="36"/>
-      <c r="X2" s="36"/>
-      <c r="Y2" s="37"/>
+      <c r="W2" s="33"/>
+      <c r="X2" s="33"/>
+      <c r="Y2" s="34"/>
       <c r="Z2" s="16"/>
-      <c r="AA2" s="35" t="s">
+      <c r="AA2" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="AB2" s="36"/>
-      <c r="AC2" s="36"/>
-      <c r="AD2" s="36"/>
-      <c r="AE2" s="36"/>
-      <c r="AF2" s="36"/>
-      <c r="AG2" s="37"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="33"/>
+      <c r="AF2" s="33"/>
+      <c r="AG2" s="34"/>
       <c r="AH2" s="17"/>
       <c r="AI2" s="19" t="s">
         <v>8</v>
@@ -1183,22 +1203,22 @@
       <c r="AP2" s="20"/>
     </row>
     <row r="3" spans="2:67" s="9" customFormat="1" ht="40.049999999999997" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="26" t="s">
         <v>24</v>
       </c>
       <c r="H3" s="18" t="s">
@@ -1225,12 +1245,12 @@
       <c r="AA3" s="8"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="27"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1414,7 +1434,7 @@
     </row>
     <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B5" s="24" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C5" s="5">
         <v>1</v>
@@ -1434,7 +1454,7 @@
     </row>
     <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B6" s="24" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="C6" s="5">
         <v>1</v>
@@ -1453,8 +1473,8 @@
       </c>
     </row>
     <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B7" s="38" t="s">
-        <v>47</v>
+      <c r="B7" s="25" t="s">
+        <v>30</v>
       </c>
       <c r="C7" s="5">
         <v>1</v>
@@ -1473,8 +1493,8 @@
       </c>
     </row>
     <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B8" s="38" t="s">
-        <v>48</v>
+      <c r="B8" s="25" t="s">
+        <v>31</v>
       </c>
       <c r="C8" s="5">
         <v>1</v>
@@ -1493,8 +1513,8 @@
       </c>
     </row>
     <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B9" s="38" t="s">
-        <v>49</v>
+      <c r="B9" s="25" t="s">
+        <v>32</v>
       </c>
       <c r="C9" s="5">
         <v>3</v>
@@ -1514,7 +1534,7 @@
     </row>
     <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B10" s="24" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="C10" s="5">
         <v>3</v>
@@ -1534,7 +1554,7 @@
     </row>
     <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B11" s="24" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C11" s="5">
         <v>4</v>
@@ -1554,7 +1574,7 @@
     </row>
     <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B12" s="24" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C12" s="5">
         <v>5</v>
@@ -1574,7 +1594,7 @@
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B13" s="24" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C13" s="5">
         <v>6</v>
@@ -1588,9 +1608,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="2:67" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B14" s="24" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C14" s="5">
         <v>9</v>
@@ -1606,7 +1626,7 @@
     </row>
     <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B15" s="24" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C15" s="5">
         <v>9</v>
@@ -1622,7 +1642,7 @@
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B16" s="24" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C16" s="5">
         <v>12</v>
@@ -1638,7 +1658,7 @@
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B17" s="24" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C17" s="6">
         <v>14</v>
@@ -1654,7 +1674,7 @@
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B18" s="24" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C18" s="5">
         <v>18</v>
@@ -1670,7 +1690,7 @@
     </row>
     <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B19" s="24" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C19" s="5">
         <v>21</v>
@@ -1686,7 +1706,7 @@
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B20" s="24" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C20" s="5">
         <v>21</v>
@@ -1702,7 +1722,7 @@
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B21" s="24" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C21" s="5">
         <v>24</v>
@@ -1718,7 +1738,7 @@
     </row>
     <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B22" s="24" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C22" s="5">
         <v>25</v>
@@ -1734,7 +1754,7 @@
     </row>
     <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B23" s="24" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C23" s="5">
         <v>26</v>
@@ -1750,7 +1770,7 @@
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B24" s="24" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C24" s="5">
         <v>27</v>
@@ -1766,7 +1786,7 @@
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B25" s="24" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C25" s="5">
         <v>27</v>
@@ -1782,7 +1802,7 @@
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B26" s="24" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C26" s="5">
         <v>30</v>
@@ -1798,7 +1818,7 @@
     </row>
     <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B27" s="24" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C27" s="5">
         <v>33</v>
@@ -1982,17 +2002,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:BO4">
     <cfRule type="expression" dxfId="8" priority="8">

</xml_diff>

<commit_message>
Updated Gantt Chart, Project Plan, and Software Design Document. idk if I need to change anymore thing for now.
</commit_message>
<xml_diff>
--- a/Gantt_chart.xlsx
+++ b/Gantt_chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\Documents\Griffith\localRepo\Milestone1_Group39\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19AA2FD-858B-4D05-83C7-09F297326F29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7FF8B7-10C7-4145-99AD-9E5C0571A5E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="1515" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17813" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -580,7 +580,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -599,9 +599,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -653,18 +650,24 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="10" applyFont="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="10" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -686,17 +689,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="10" applyFont="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1100,152 +1106,152 @@
   </sheetPr>
   <dimension ref="B1:BO41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="CJ1" sqref="CJ1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.73046875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.59765625" customWidth="1"/>
-    <col min="2" max="2" width="21.46484375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="6.59765625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.265625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="5.73046875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6.73046875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" style="4" customWidth="1"/>
-    <col min="8" max="14" width="2.73046875" style="1"/>
-    <col min="15" max="16" width="2.73046875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="3.9296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.53125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="26" width="3.9296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="3.9296875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.19921875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="4.19921875" customWidth="1"/>
-    <col min="31" max="34" width="4.19921875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="4.06640625" customWidth="1"/>
-    <col min="36" max="37" width="4.19921875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="3.9296875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="4.19921875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="4.19921875" customWidth="1"/>
-    <col min="41" max="47" width="4.19921875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="3.9296875" bestFit="1" customWidth="1"/>
-    <col min="49" max="57" width="4.19921875" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="3.9296875" bestFit="1" customWidth="1"/>
-    <col min="59" max="67" width="4.19921875" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="2.73046875" customWidth="1"/>
+    <col min="1" max="1" width="2.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.35546875" style="4" customWidth="1"/>
+    <col min="8" max="14" width="2.7109375" style="1"/>
+    <col min="15" max="16" width="2.7109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="3.92578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="26" width="3.92578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.2109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3.92578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="4.2109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="4.2109375" customWidth="1"/>
+    <col min="31" max="34" width="4.2109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="4.0703125" customWidth="1"/>
+    <col min="36" max="37" width="4.2109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="3.92578125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="4.2109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="4.2109375" customWidth="1"/>
+    <col min="41" max="47" width="4.2109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="3.92578125" bestFit="1" customWidth="1"/>
+    <col min="49" max="57" width="4.2109375" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="3.92578125" bestFit="1" customWidth="1"/>
+    <col min="59" max="67" width="4.2109375" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.6">
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.4">
+      <c r="B1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-    </row>
-    <row r="2" spans="2:67" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="21" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+    </row>
+    <row r="2" spans="2:67" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="12">
+      <c r="H2" s="11">
+        <v>11</v>
+      </c>
+      <c r="J2" s="12"/>
+      <c r="K2" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="13"/>
-      <c r="K2" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="W2" s="33"/>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="34"/>
-      <c r="Z2" s="16"/>
-      <c r="AA2" s="32" t="s">
+      <c r="W2" s="34"/>
+      <c r="X2" s="34"/>
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="AB2" s="33"/>
-      <c r="AC2" s="33"/>
-      <c r="AD2" s="33"/>
-      <c r="AE2" s="33"/>
-      <c r="AF2" s="33"/>
-      <c r="AG2" s="34"/>
-      <c r="AH2" s="17"/>
-      <c r="AI2" s="19" t="s">
+      <c r="AB2" s="34"/>
+      <c r="AC2" s="34"/>
+      <c r="AD2" s="34"/>
+      <c r="AE2" s="34"/>
+      <c r="AF2" s="34"/>
+      <c r="AG2" s="35"/>
+      <c r="AH2" s="16"/>
+      <c r="AI2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="AJ2" s="20"/>
-      <c r="AK2" s="20"/>
-      <c r="AL2" s="20"/>
-      <c r="AM2" s="20"/>
-      <c r="AN2" s="20"/>
-      <c r="AO2" s="20"/>
-      <c r="AP2" s="20"/>
-    </row>
-    <row r="3" spans="2:67" s="9" customFormat="1" ht="40.049999999999997" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="36" t="s">
+      <c r="AJ2" s="19"/>
+      <c r="AK2" s="19"/>
+      <c r="AL2" s="19"/>
+      <c r="AM2" s="19"/>
+      <c r="AN2" s="19"/>
+      <c r="AO2" s="19"/>
+      <c r="AP2" s="19"/>
+    </row>
+    <row r="3" spans="2:67" s="8" customFormat="1" ht="40.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-    </row>
-    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="37"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+    </row>
+    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="25"/>
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
       <c r="E4" s="27"/>
@@ -1432,587 +1438,623 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="24" t="s">
+    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="5">
-        <v>1</v>
-      </c>
-      <c r="E5" s="5">
-        <v>1</v>
-      </c>
-      <c r="F5" s="5">
-        <v>1</v>
-      </c>
-      <c r="G5" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="24" t="s">
+      <c r="C5" s="37">
+        <v>1</v>
+      </c>
+      <c r="D5" s="37">
+        <v>1</v>
+      </c>
+      <c r="E5" s="37">
+        <v>1</v>
+      </c>
+      <c r="F5" s="37">
+        <v>1</v>
+      </c>
+      <c r="G5" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="5">
-        <v>1</v>
-      </c>
-      <c r="D6" s="5">
+      <c r="C6" s="37">
+        <v>1</v>
+      </c>
+      <c r="D6" s="37">
         <v>3</v>
       </c>
-      <c r="E6" s="5">
-        <v>1</v>
-      </c>
-      <c r="F6" s="5">
+      <c r="E6" s="37">
+        <v>1</v>
+      </c>
+      <c r="F6" s="37">
         <v>3</v>
       </c>
-      <c r="G6" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B7" s="25" t="s">
+      <c r="G6" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="5">
-        <v>1</v>
-      </c>
-      <c r="D7" s="5">
-        <v>1</v>
-      </c>
-      <c r="E7" s="5">
-        <v>1</v>
-      </c>
-      <c r="F7" s="5">
-        <v>1</v>
-      </c>
-      <c r="G7" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B8" s="25" t="s">
+      <c r="C7" s="37">
+        <v>1</v>
+      </c>
+      <c r="D7" s="37">
+        <v>1</v>
+      </c>
+      <c r="E7" s="37">
+        <v>1</v>
+      </c>
+      <c r="F7" s="37">
+        <v>1</v>
+      </c>
+      <c r="G7" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="5">
-        <v>1</v>
-      </c>
-      <c r="D8" s="5">
-        <v>1</v>
-      </c>
-      <c r="E8" s="5">
-        <v>1</v>
-      </c>
-      <c r="F8" s="5">
-        <v>1</v>
-      </c>
-      <c r="G8" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B9" s="25" t="s">
+      <c r="C8" s="37">
+        <v>1</v>
+      </c>
+      <c r="D8" s="37">
+        <v>1</v>
+      </c>
+      <c r="E8" s="37">
+        <v>1</v>
+      </c>
+      <c r="F8" s="37">
+        <v>1</v>
+      </c>
+      <c r="G8" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="37">
         <v>3</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="37">
         <v>4</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="37">
         <v>3</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="37">
         <v>4</v>
       </c>
-      <c r="G9" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B10" s="24" t="s">
+      <c r="G9" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="37">
         <v>3</v>
       </c>
-      <c r="D10" s="5">
-        <v>1</v>
-      </c>
-      <c r="E10" s="5">
+      <c r="D10" s="37">
+        <v>1</v>
+      </c>
+      <c r="E10" s="37">
         <v>3</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="37">
         <v>2</v>
       </c>
-      <c r="G10" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B11" s="24" t="s">
+      <c r="G10" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="37">
         <v>4</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="37">
         <v>2</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="37">
         <v>4</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="37">
         <v>2</v>
       </c>
-      <c r="G11" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B12" s="24" t="s">
+      <c r="G11" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="37">
         <v>5</v>
       </c>
-      <c r="D12" s="5">
-        <v>1</v>
-      </c>
-      <c r="E12" s="5">
+      <c r="D12" s="37">
+        <v>1</v>
+      </c>
+      <c r="E12" s="37">
         <v>5</v>
       </c>
-      <c r="F12" s="5">
-        <v>1</v>
-      </c>
-      <c r="G12" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B13" s="24" t="s">
+      <c r="F12" s="37">
+        <v>1</v>
+      </c>
+      <c r="G12" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="37">
         <v>6</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="37">
         <v>3</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="22">
+      <c r="E13" s="37">
+        <v>6</v>
+      </c>
+      <c r="F13" s="37">
+        <v>1</v>
+      </c>
+      <c r="G13" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:67" ht="31.75" x14ac:dyDescent="0.4">
+      <c r="B14" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="37">
+        <v>9</v>
+      </c>
+      <c r="D14" s="37">
+        <v>3</v>
+      </c>
+      <c r="E14" s="37">
+        <v>6</v>
+      </c>
+      <c r="F14" s="37">
+        <v>1</v>
+      </c>
+      <c r="G14" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="37">
+        <v>9</v>
+      </c>
+      <c r="D15" s="37">
+        <v>2</v>
+      </c>
+      <c r="E15" s="37">
+        <v>7</v>
+      </c>
+      <c r="F15" s="37">
+        <v>1</v>
+      </c>
+      <c r="G15" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="37">
+        <v>12</v>
+      </c>
+      <c r="D16" s="37">
+        <v>2</v>
+      </c>
+      <c r="E16" s="37">
+        <v>7</v>
+      </c>
+      <c r="F16" s="37">
+        <v>1</v>
+      </c>
+      <c r="G16" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="40">
+        <v>14</v>
+      </c>
+      <c r="D17" s="37">
+        <v>4</v>
+      </c>
+      <c r="E17" s="37">
+        <v>8</v>
+      </c>
+      <c r="F17" s="37">
+        <v>1</v>
+      </c>
+      <c r="G17" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="37">
+        <v>18</v>
+      </c>
+      <c r="D18" s="37">
+        <v>3</v>
+      </c>
+      <c r="E18" s="37">
+        <v>9</v>
+      </c>
+      <c r="F18" s="37">
+        <v>3</v>
+      </c>
+      <c r="G18" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="37">
+        <v>21</v>
+      </c>
+      <c r="D19" s="37">
+        <v>2</v>
+      </c>
+      <c r="E19" s="37">
+        <v>9</v>
+      </c>
+      <c r="F19" s="37">
+        <v>3</v>
+      </c>
+      <c r="G19" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="37">
+        <v>21</v>
+      </c>
+      <c r="D20" s="37">
+        <v>3</v>
+      </c>
+      <c r="E20" s="37">
+        <v>9</v>
+      </c>
+      <c r="F20" s="37">
+        <v>3</v>
+      </c>
+      <c r="G20" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="37">
+        <v>24</v>
+      </c>
+      <c r="D21" s="37">
+        <v>1</v>
+      </c>
+      <c r="E21" s="37">
+        <v>11</v>
+      </c>
+      <c r="F21" s="37">
+        <v>1</v>
+      </c>
+      <c r="G21" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="37">
+        <v>25</v>
+      </c>
+      <c r="D22" s="37">
+        <v>1</v>
+      </c>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="38">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:67" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="B14" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="5">
-        <v>9</v>
-      </c>
-      <c r="D14" s="5">
+    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="37">
+        <v>26</v>
+      </c>
+      <c r="D23" s="37">
+        <v>1</v>
+      </c>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B24" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="37">
+        <v>27</v>
+      </c>
+      <c r="D24" s="37">
         <v>3</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="22">
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="38">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B15" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="5">
-        <v>9</v>
-      </c>
-      <c r="D15" s="5">
+    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="37">
+        <v>27</v>
+      </c>
+      <c r="D25" s="37">
         <v>2</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="22">
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="38">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B16" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="5">
-        <v>12</v>
-      </c>
-      <c r="D16" s="5">
+    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="37">
+        <v>30</v>
+      </c>
+      <c r="D26" s="37">
+        <v>3</v>
+      </c>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B27" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="37">
+        <v>33</v>
+      </c>
+      <c r="D27" s="37">
         <v>2</v>
       </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="22">
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="38">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B17" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="6">
-        <v>14</v>
-      </c>
-      <c r="D17" s="5">
-        <v>4</v>
-      </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B18" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="5">
-        <v>18</v>
-      </c>
-      <c r="D18" s="5">
-        <v>3</v>
-      </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B19" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="5">
-        <v>21</v>
-      </c>
-      <c r="D19" s="5">
-        <v>2</v>
-      </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B20" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="5">
-        <v>21</v>
-      </c>
-      <c r="D20" s="5">
-        <v>3</v>
-      </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B21" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="5">
-        <v>24</v>
-      </c>
-      <c r="D21" s="5">
-        <v>1</v>
-      </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B22" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="5">
-        <v>25</v>
-      </c>
-      <c r="D22" s="5">
-        <v>1</v>
-      </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B23" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="5">
-        <v>26</v>
-      </c>
-      <c r="D23" s="5">
-        <v>1</v>
-      </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B24" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="5">
-        <v>27</v>
-      </c>
-      <c r="D24" s="5">
-        <v>3</v>
-      </c>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B25" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="5">
-        <v>27</v>
-      </c>
-      <c r="D25" s="5">
-        <v>2</v>
-      </c>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B26" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="5">
-        <v>30</v>
-      </c>
-      <c r="D26" s="5">
-        <v>3</v>
-      </c>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B27" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="5">
-        <v>33</v>
-      </c>
-      <c r="D27" s="5">
-        <v>2</v>
-      </c>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B28" s="23" t="s">
+    <row r="28" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B28" s="22" t="s">
         <v>1</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
-      <c r="G28" s="22">
+      <c r="G28" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B29" s="23" t="s">
+    <row r="29" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B29" s="22" t="s">
         <v>2</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
-      <c r="G29" s="22">
+      <c r="G29" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B30" s="23" t="s">
+    <row r="30" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B30" s="22" t="s">
         <v>3</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
-      <c r="G30" s="22">
+      <c r="G30" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B31" s="23" t="s">
+    <row r="31" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B31" s="22" t="s">
         <v>4</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
-      <c r="G31" s="22">
+      <c r="G31" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B32" s="23" t="s">
+    <row r="32" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B32" s="22" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
-      <c r="G32" s="22">
+      <c r="G32" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B33" s="23" t="s">
+    <row r="33" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B33" s="22" t="s">
         <v>11</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
-      <c r="G33" s="22">
+      <c r="G33" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B34" s="23" t="s">
+    <row r="34" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B34" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
-      <c r="G34" s="22">
+      <c r="G34" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B35" s="23" t="s">
+    <row r="35" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B35" s="22" t="s">
         <v>13</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
-      <c r="G35" s="22">
+      <c r="G35" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B36" s="23" t="s">
+    <row r="36" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B36" s="22" t="s">
         <v>14</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
-      <c r="G36" s="22">
+      <c r="G36" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B37" s="23" t="s">
+    <row r="37" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B37" s="22" t="s">
         <v>15</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
-      <c r="G37" s="22">
+      <c r="G37" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B38" s="23" t="s">
+    <row r="38" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B38" s="22" t="s">
         <v>16</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
-      <c r="G38" s="22">
+      <c r="G38" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B39" s="23" t="s">
+    <row r="39" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B39" s="22" t="s">
         <v>17</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
-      <c r="G39" s="22">
+      <c r="G39" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B40" s="23" t="s">
+    <row r="40" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B40" s="22" t="s">
         <v>18</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
-      <c r="G40" s="22">
+      <c r="G40" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B41" s="23" t="s">
+    <row r="41" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B41" s="22" t="s">
         <v>19</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
-      <c r="G41" s="22">
+      <c r="G41" s="21">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:BO4">
     <cfRule type="expression" dxfId="8" priority="8">

</xml_diff>

<commit_message>
idk whats happening here
</commit_message>
<xml_diff>
--- a/Gantt_chart.xlsx
+++ b/Gantt_chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\Documents\Griffith\localRepo\Milestone1_Group39\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19AA2FD-858B-4D05-83C7-09F297326F29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7FF8B7-10C7-4145-99AD-9E5C0571A5E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="1515" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17813" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -580,7 +580,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -599,9 +599,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -653,18 +650,24 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="10" applyFont="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="10" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -686,17 +689,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="10" applyFont="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1100,152 +1106,152 @@
   </sheetPr>
   <dimension ref="B1:BO41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="CJ1" sqref="CJ1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.73046875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.59765625" customWidth="1"/>
-    <col min="2" max="2" width="21.46484375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="6.59765625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.265625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="5.73046875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6.73046875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" style="4" customWidth="1"/>
-    <col min="8" max="14" width="2.73046875" style="1"/>
-    <col min="15" max="16" width="2.73046875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="3.9296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.53125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="26" width="3.9296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="3.9296875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.19921875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="4.19921875" customWidth="1"/>
-    <col min="31" max="34" width="4.19921875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="4.06640625" customWidth="1"/>
-    <col min="36" max="37" width="4.19921875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="3.9296875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="4.19921875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="4.19921875" customWidth="1"/>
-    <col min="41" max="47" width="4.19921875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="3.9296875" bestFit="1" customWidth="1"/>
-    <col min="49" max="57" width="4.19921875" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="3.9296875" bestFit="1" customWidth="1"/>
-    <col min="59" max="67" width="4.19921875" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="2.73046875" customWidth="1"/>
+    <col min="1" max="1" width="2.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.35546875" style="4" customWidth="1"/>
+    <col min="8" max="14" width="2.7109375" style="1"/>
+    <col min="15" max="16" width="2.7109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="3.92578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="26" width="3.92578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.2109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3.92578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="4.2109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="4.2109375" customWidth="1"/>
+    <col min="31" max="34" width="4.2109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="4.0703125" customWidth="1"/>
+    <col min="36" max="37" width="4.2109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="3.92578125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="4.2109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="4.2109375" customWidth="1"/>
+    <col min="41" max="47" width="4.2109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="3.92578125" bestFit="1" customWidth="1"/>
+    <col min="49" max="57" width="4.2109375" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="3.92578125" bestFit="1" customWidth="1"/>
+    <col min="59" max="67" width="4.2109375" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.6">
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.4">
+      <c r="B1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-    </row>
-    <row r="2" spans="2:67" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="21" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+    </row>
+    <row r="2" spans="2:67" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="12">
+      <c r="H2" s="11">
+        <v>11</v>
+      </c>
+      <c r="J2" s="12"/>
+      <c r="K2" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="13"/>
-      <c r="K2" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="W2" s="33"/>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="34"/>
-      <c r="Z2" s="16"/>
-      <c r="AA2" s="32" t="s">
+      <c r="W2" s="34"/>
+      <c r="X2" s="34"/>
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="AB2" s="33"/>
-      <c r="AC2" s="33"/>
-      <c r="AD2" s="33"/>
-      <c r="AE2" s="33"/>
-      <c r="AF2" s="33"/>
-      <c r="AG2" s="34"/>
-      <c r="AH2" s="17"/>
-      <c r="AI2" s="19" t="s">
+      <c r="AB2" s="34"/>
+      <c r="AC2" s="34"/>
+      <c r="AD2" s="34"/>
+      <c r="AE2" s="34"/>
+      <c r="AF2" s="34"/>
+      <c r="AG2" s="35"/>
+      <c r="AH2" s="16"/>
+      <c r="AI2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="AJ2" s="20"/>
-      <c r="AK2" s="20"/>
-      <c r="AL2" s="20"/>
-      <c r="AM2" s="20"/>
-      <c r="AN2" s="20"/>
-      <c r="AO2" s="20"/>
-      <c r="AP2" s="20"/>
-    </row>
-    <row r="3" spans="2:67" s="9" customFormat="1" ht="40.049999999999997" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="36" t="s">
+      <c r="AJ2" s="19"/>
+      <c r="AK2" s="19"/>
+      <c r="AL2" s="19"/>
+      <c r="AM2" s="19"/>
+      <c r="AN2" s="19"/>
+      <c r="AO2" s="19"/>
+      <c r="AP2" s="19"/>
+    </row>
+    <row r="3" spans="2:67" s="8" customFormat="1" ht="40.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-    </row>
-    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="37"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+    </row>
+    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="25"/>
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
       <c r="E4" s="27"/>
@@ -1432,587 +1438,623 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="24" t="s">
+    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="5">
-        <v>1</v>
-      </c>
-      <c r="E5" s="5">
-        <v>1</v>
-      </c>
-      <c r="F5" s="5">
-        <v>1</v>
-      </c>
-      <c r="G5" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="24" t="s">
+      <c r="C5" s="37">
+        <v>1</v>
+      </c>
+      <c r="D5" s="37">
+        <v>1</v>
+      </c>
+      <c r="E5" s="37">
+        <v>1</v>
+      </c>
+      <c r="F5" s="37">
+        <v>1</v>
+      </c>
+      <c r="G5" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="5">
-        <v>1</v>
-      </c>
-      <c r="D6" s="5">
+      <c r="C6" s="37">
+        <v>1</v>
+      </c>
+      <c r="D6" s="37">
         <v>3</v>
       </c>
-      <c r="E6" s="5">
-        <v>1</v>
-      </c>
-      <c r="F6" s="5">
+      <c r="E6" s="37">
+        <v>1</v>
+      </c>
+      <c r="F6" s="37">
         <v>3</v>
       </c>
-      <c r="G6" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B7" s="25" t="s">
+      <c r="G6" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="5">
-        <v>1</v>
-      </c>
-      <c r="D7" s="5">
-        <v>1</v>
-      </c>
-      <c r="E7" s="5">
-        <v>1</v>
-      </c>
-      <c r="F7" s="5">
-        <v>1</v>
-      </c>
-      <c r="G7" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B8" s="25" t="s">
+      <c r="C7" s="37">
+        <v>1</v>
+      </c>
+      <c r="D7" s="37">
+        <v>1</v>
+      </c>
+      <c r="E7" s="37">
+        <v>1</v>
+      </c>
+      <c r="F7" s="37">
+        <v>1</v>
+      </c>
+      <c r="G7" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="5">
-        <v>1</v>
-      </c>
-      <c r="D8" s="5">
-        <v>1</v>
-      </c>
-      <c r="E8" s="5">
-        <v>1</v>
-      </c>
-      <c r="F8" s="5">
-        <v>1</v>
-      </c>
-      <c r="G8" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B9" s="25" t="s">
+      <c r="C8" s="37">
+        <v>1</v>
+      </c>
+      <c r="D8" s="37">
+        <v>1</v>
+      </c>
+      <c r="E8" s="37">
+        <v>1</v>
+      </c>
+      <c r="F8" s="37">
+        <v>1</v>
+      </c>
+      <c r="G8" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="37">
         <v>3</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="37">
         <v>4</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="37">
         <v>3</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="37">
         <v>4</v>
       </c>
-      <c r="G9" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B10" s="24" t="s">
+      <c r="G9" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="37">
         <v>3</v>
       </c>
-      <c r="D10" s="5">
-        <v>1</v>
-      </c>
-      <c r="E10" s="5">
+      <c r="D10" s="37">
+        <v>1</v>
+      </c>
+      <c r="E10" s="37">
         <v>3</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="37">
         <v>2</v>
       </c>
-      <c r="G10" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B11" s="24" t="s">
+      <c r="G10" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="37">
         <v>4</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="37">
         <v>2</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="37">
         <v>4</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="37">
         <v>2</v>
       </c>
-      <c r="G11" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B12" s="24" t="s">
+      <c r="G11" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="37">
         <v>5</v>
       </c>
-      <c r="D12" s="5">
-        <v>1</v>
-      </c>
-      <c r="E12" s="5">
+      <c r="D12" s="37">
+        <v>1</v>
+      </c>
+      <c r="E12" s="37">
         <v>5</v>
       </c>
-      <c r="F12" s="5">
-        <v>1</v>
-      </c>
-      <c r="G12" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B13" s="24" t="s">
+      <c r="F12" s="37">
+        <v>1</v>
+      </c>
+      <c r="G12" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="37">
         <v>6</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="37">
         <v>3</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="22">
+      <c r="E13" s="37">
+        <v>6</v>
+      </c>
+      <c r="F13" s="37">
+        <v>1</v>
+      </c>
+      <c r="G13" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:67" ht="31.75" x14ac:dyDescent="0.4">
+      <c r="B14" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="37">
+        <v>9</v>
+      </c>
+      <c r="D14" s="37">
+        <v>3</v>
+      </c>
+      <c r="E14" s="37">
+        <v>6</v>
+      </c>
+      <c r="F14" s="37">
+        <v>1</v>
+      </c>
+      <c r="G14" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="37">
+        <v>9</v>
+      </c>
+      <c r="D15" s="37">
+        <v>2</v>
+      </c>
+      <c r="E15" s="37">
+        <v>7</v>
+      </c>
+      <c r="F15" s="37">
+        <v>1</v>
+      </c>
+      <c r="G15" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="37">
+        <v>12</v>
+      </c>
+      <c r="D16" s="37">
+        <v>2</v>
+      </c>
+      <c r="E16" s="37">
+        <v>7</v>
+      </c>
+      <c r="F16" s="37">
+        <v>1</v>
+      </c>
+      <c r="G16" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="40">
+        <v>14</v>
+      </c>
+      <c r="D17" s="37">
+        <v>4</v>
+      </c>
+      <c r="E17" s="37">
+        <v>8</v>
+      </c>
+      <c r="F17" s="37">
+        <v>1</v>
+      </c>
+      <c r="G17" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="37">
+        <v>18</v>
+      </c>
+      <c r="D18" s="37">
+        <v>3</v>
+      </c>
+      <c r="E18" s="37">
+        <v>9</v>
+      </c>
+      <c r="F18" s="37">
+        <v>3</v>
+      </c>
+      <c r="G18" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="37">
+        <v>21</v>
+      </c>
+      <c r="D19" s="37">
+        <v>2</v>
+      </c>
+      <c r="E19" s="37">
+        <v>9</v>
+      </c>
+      <c r="F19" s="37">
+        <v>3</v>
+      </c>
+      <c r="G19" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="37">
+        <v>21</v>
+      </c>
+      <c r="D20" s="37">
+        <v>3</v>
+      </c>
+      <c r="E20" s="37">
+        <v>9</v>
+      </c>
+      <c r="F20" s="37">
+        <v>3</v>
+      </c>
+      <c r="G20" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="37">
+        <v>24</v>
+      </c>
+      <c r="D21" s="37">
+        <v>1</v>
+      </c>
+      <c r="E21" s="37">
+        <v>11</v>
+      </c>
+      <c r="F21" s="37">
+        <v>1</v>
+      </c>
+      <c r="G21" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="37">
+        <v>25</v>
+      </c>
+      <c r="D22" s="37">
+        <v>1</v>
+      </c>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="38">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:67" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="B14" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="5">
-        <v>9</v>
-      </c>
-      <c r="D14" s="5">
+    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="37">
+        <v>26</v>
+      </c>
+      <c r="D23" s="37">
+        <v>1</v>
+      </c>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B24" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="37">
+        <v>27</v>
+      </c>
+      <c r="D24" s="37">
         <v>3</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="22">
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="38">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B15" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="5">
-        <v>9</v>
-      </c>
-      <c r="D15" s="5">
+    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="37">
+        <v>27</v>
+      </c>
+      <c r="D25" s="37">
         <v>2</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="22">
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="38">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B16" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="5">
-        <v>12</v>
-      </c>
-      <c r="D16" s="5">
+    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="37">
+        <v>30</v>
+      </c>
+      <c r="D26" s="37">
+        <v>3</v>
+      </c>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B27" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="37">
+        <v>33</v>
+      </c>
+      <c r="D27" s="37">
         <v>2</v>
       </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="22">
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="38">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B17" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="6">
-        <v>14</v>
-      </c>
-      <c r="D17" s="5">
-        <v>4</v>
-      </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B18" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="5">
-        <v>18</v>
-      </c>
-      <c r="D18" s="5">
-        <v>3</v>
-      </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B19" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="5">
-        <v>21</v>
-      </c>
-      <c r="D19" s="5">
-        <v>2</v>
-      </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B20" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="5">
-        <v>21</v>
-      </c>
-      <c r="D20" s="5">
-        <v>3</v>
-      </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B21" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="5">
-        <v>24</v>
-      </c>
-      <c r="D21" s="5">
-        <v>1</v>
-      </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B22" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="5">
-        <v>25</v>
-      </c>
-      <c r="D22" s="5">
-        <v>1</v>
-      </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B23" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="5">
-        <v>26</v>
-      </c>
-      <c r="D23" s="5">
-        <v>1</v>
-      </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B24" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="5">
-        <v>27</v>
-      </c>
-      <c r="D24" s="5">
-        <v>3</v>
-      </c>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B25" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="5">
-        <v>27</v>
-      </c>
-      <c r="D25" s="5">
-        <v>2</v>
-      </c>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B26" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="5">
-        <v>30</v>
-      </c>
-      <c r="D26" s="5">
-        <v>3</v>
-      </c>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B27" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="5">
-        <v>33</v>
-      </c>
-      <c r="D27" s="5">
-        <v>2</v>
-      </c>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B28" s="23" t="s">
+    <row r="28" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B28" s="22" t="s">
         <v>1</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
-      <c r="G28" s="22">
+      <c r="G28" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B29" s="23" t="s">
+    <row r="29" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B29" s="22" t="s">
         <v>2</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
-      <c r="G29" s="22">
+      <c r="G29" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B30" s="23" t="s">
+    <row r="30" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B30" s="22" t="s">
         <v>3</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
-      <c r="G30" s="22">
+      <c r="G30" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B31" s="23" t="s">
+    <row r="31" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B31" s="22" t="s">
         <v>4</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
-      <c r="G31" s="22">
+      <c r="G31" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B32" s="23" t="s">
+    <row r="32" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B32" s="22" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
-      <c r="G32" s="22">
+      <c r="G32" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B33" s="23" t="s">
+    <row r="33" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B33" s="22" t="s">
         <v>11</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
-      <c r="G33" s="22">
+      <c r="G33" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B34" s="23" t="s">
+    <row r="34" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B34" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
-      <c r="G34" s="22">
+      <c r="G34" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B35" s="23" t="s">
+    <row r="35" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B35" s="22" t="s">
         <v>13</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
-      <c r="G35" s="22">
+      <c r="G35" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B36" s="23" t="s">
+    <row r="36" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B36" s="22" t="s">
         <v>14</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
-      <c r="G36" s="22">
+      <c r="G36" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B37" s="23" t="s">
+    <row r="37" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B37" s="22" t="s">
         <v>15</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
-      <c r="G37" s="22">
+      <c r="G37" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B38" s="23" t="s">
+    <row r="38" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B38" s="22" t="s">
         <v>16</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
-      <c r="G38" s="22">
+      <c r="G38" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B39" s="23" t="s">
+    <row r="39" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B39" s="22" t="s">
         <v>17</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
-      <c r="G39" s="22">
+      <c r="G39" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B40" s="23" t="s">
+    <row r="40" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B40" s="22" t="s">
         <v>18</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
-      <c r="G40" s="22">
+      <c r="G40" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B41" s="23" t="s">
+    <row r="41" spans="2:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B41" s="22" t="s">
         <v>19</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
-      <c r="G41" s="22">
+      <c r="G41" s="21">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:BO4">
     <cfRule type="expression" dxfId="8" priority="8">

</xml_diff>